<commit_message>
20250907-1155;chybu som spôsil ja tým že do bunky sm dal 3 riadky. Prerobili sme generator, strankujeme prehľady, upravené ikony, pozadie na hnede. Otestované na lokali.
</commit_message>
<xml_diff>
--- a/docs/sk/KNIFES/K064-ga4-gtn-utm/GA4andGTM/UTM_Generator_Template_with_Formula.xlsx
+++ b/docs/sk/KNIFES/K064-ga4-gtn-utm/GA4andGTM/UTM_Generator_Template_with_Formula.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romankazicka/Documents/800-CAS-ContextAwareApproach/06-STH-Projects/class_system_thinking_in_it/docs/sk/01.KnowledgeContributions/01-Marketing/GA4andGTM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romankazicka/Documents/800-CAS-ContextAwareApproach/03-KNIFE-Framework/knifes_overviews-02/docs/sk/knifes/K064-ga4-gtn-utm/GA4andGTM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10A3077-C040-0C4B-BEE0-D5DBF7DC1423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D561B81-561D-1846-878D-00971D68713F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Base URL</t>
   </si>
@@ -66,16 +66,30 @@
   </si>
   <si>
     <t>button1</t>
+  </si>
+  <si>
+    <t>https://sthdf.systemthinking.sk</t>
+  </si>
+  <si>
+    <t>repost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,13 +112,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,7 +425,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -461,9 +478,18 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
-        <v>?utm_source=&amp;utm_medium=&amp;utm_campaign=&amp;utm_content=</v>
+        <v>https://sthdf.systemthinking.sk?utm_source=linkedin&amp;utm_medium=repost&amp;utm_campaign=&amp;utm_content=</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1032,7 +1058,7 @@
     </row>
     <row r="98" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F98" t="str">
-        <f t="shared" ref="F98:F129" si="3">A98 &amp; "?utm_source=" &amp; B98 &amp; "&amp;utm_medium=" &amp; C98 &amp; "&amp;utm_campaign=" &amp; D98 &amp; "&amp;utm_content=" &amp; E98</f>
+        <f t="shared" ref="F98:F101" si="3">A98 &amp; "?utm_source=" &amp; B98 &amp; "&amp;utm_medium=" &amp; C98 &amp; "&amp;utm_campaign=" &amp; D98 &amp; "&amp;utm_content=" &amp; E98</f>
         <v>?utm_source=&amp;utm_medium=&amp;utm_campaign=&amp;utm_content=</v>
       </c>
     </row>
@@ -1055,6 +1081,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{F27C9F02-230A-2E4F-A778-CC016B709D7B}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>